<commit_message>
260122 DataBase Auth 컬럼 확장
</commit_message>
<xml_diff>
--- a/db/DataBaseCol.xlsx
+++ b/db/DataBaseCol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\251128_물품보관함\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\TeamProjectStraffic_\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6C75CAF-BF41-4F75-BAB1-672A74463B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A79B49-797B-455C-95D2-07348A4D438E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="15720" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
   </bookViews>
@@ -293,7 +293,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>권한(1: Master 2: 운영자 3: 대기)</t>
+    <t>권한(1: Master 2: 운영자 3: 대기 4: 비활성화)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A039B4-B4EC-499B-B846-66B839DA3680}">
   <dimension ref="B2:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -709,7 +709,7 @@
     <col min="3" max="3" width="15.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
260129 Incident station_id  cancel  Notnull
</commit_message>
<xml_diff>
--- a/db/DataBaseCol.xlsx
+++ b/db/DataBaseCol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\SAP_Straffic260119\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8189E177-8CD2-4417-9F1F-5D47397C8764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933DED3D-7061-47AE-8263-A6461F0EA283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{008F3ED9-E954-48A9-9E03-D39CBFFCB847}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="104">
   <si>
     <t>DB</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A039B4-B4EC-499B-B846-66B839DA3680}">
   <dimension ref="B2:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1514,9 +1514,7 @@
         <v>95</v>
       </c>
       <c r="D49" s="1"/>
-      <c r="E49" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>